<commit_message>
Final weight entered and working on redoing PWG and SGR
</commit_message>
<xml_diff>
--- a/Raw_data.xlsx
+++ b/Raw_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lasse\Analysis Git\Methionine experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B813D8E5-9338-49E2-9F63-50814EC5F9EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B42688E-76C0-4A9E-ADA0-41005D980F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3735" yWindow="2737" windowWidth="16200" windowHeight="8483" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-83" yWindow="0" windowWidth="10965" windowHeight="12863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="14">
   <si>
     <t>Tmt</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>Met</t>
   </si>
 </sst>
 </file>
@@ -387,236 +390,275 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E106"/>
+  <dimension ref="A1:F148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="H126" sqref="H126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
         <v>0</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
       <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>0.4</v>
       </c>
       <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
         <v>0</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>0.99</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>0.4</v>
       </c>
       <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
         <v>0</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>1.23</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
         <v>0</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>1.03</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
         <v>0</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>0.88</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
         <v>0</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>1.29</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
         <v>0</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>1.03</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>0.7</v>
       </c>
       <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
         <v>0</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>1.01</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>0.7</v>
       </c>
       <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
         <v>0</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>1.2</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>5</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>0.85</v>
       </c>
       <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
         <v>0</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>1.02</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>5</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>0.85</v>
       </c>
       <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
         <v>0</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>1.05</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>5</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>0.85</v>
       </c>
       <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
         <v>0</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>1.26</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -624,356 +666,419 @@
         <v>1</v>
       </c>
       <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
         <v>0</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>1.08</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>6</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
         <v>0</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>1.23</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>6</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
         <v>0</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>1.1499999999999999</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>7</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
         <v>0</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>1.02</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>7</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
         <v>0</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>1.1399999999999999</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>7</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
         <v>0</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>1.1200000000000001</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>8</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
         <v>0</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>1.02</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>8</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>1.3</v>
       </c>
       <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
         <v>0</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>1.07</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>8</v>
       </c>
       <c r="B22">
-        <v>3</v>
+        <v>1.3</v>
       </c>
       <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22">
         <v>0</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>1.35</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>2</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
-      <c r="D23" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23">
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>2</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>0.4</v>
       </c>
       <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>2</v>
       </c>
       <c r="B25">
-        <v>3</v>
+        <v>0.4</v>
       </c>
       <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>3</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="D26" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26">
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>3</v>
       </c>
       <c r="B27">
-        <v>2</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27" t="s">
-        <v>12</v>
-      </c>
-      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27">
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>3</v>
       </c>
       <c r="B28">
-        <v>3</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C28">
-        <v>1</v>
-      </c>
-      <c r="D28" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28">
+        <v>3</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>4</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
-      <c r="D29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E29">
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29">
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>4</v>
       </c>
       <c r="B30">
-        <v>2</v>
+        <v>0.7</v>
       </c>
       <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>4</v>
       </c>
       <c r="B31">
-        <v>3</v>
+        <v>0.7</v>
       </c>
       <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="D31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E31">
+        <v>3</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31">
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>5</v>
       </c>
       <c r="B32">
-        <v>1</v>
+        <v>0.85</v>
       </c>
       <c r="C32">
         <v>1</v>
       </c>
-      <c r="D32" t="s">
-        <v>12</v>
-      </c>
-      <c r="E32">
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32">
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>5</v>
       </c>
       <c r="B33">
-        <v>2</v>
+        <v>0.85</v>
       </c>
       <c r="C33">
-        <v>1</v>
-      </c>
-      <c r="D33" t="s">
-        <v>12</v>
-      </c>
-      <c r="E33">
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33">
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>5</v>
       </c>
       <c r="B34">
-        <v>3</v>
+        <v>0.85</v>
       </c>
       <c r="C34">
-        <v>1</v>
-      </c>
-      <c r="D34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E34">
+        <v>3</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34">
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -983,354 +1088,417 @@
       <c r="C35">
         <v>1</v>
       </c>
-      <c r="D35" t="s">
-        <v>12</v>
-      </c>
-      <c r="E35">
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35">
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>6</v>
       </c>
       <c r="B36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C36">
-        <v>1</v>
-      </c>
-      <c r="D36" t="s">
-        <v>12</v>
-      </c>
-      <c r="E36">
+        <v>2</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36">
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>6</v>
       </c>
       <c r="B37">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C37">
-        <v>1</v>
-      </c>
-      <c r="D37" t="s">
-        <v>12</v>
-      </c>
-      <c r="E37">
+        <v>3</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37">
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>7</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="C38">
         <v>1</v>
       </c>
-      <c r="D38" t="s">
-        <v>12</v>
-      </c>
-      <c r="E38">
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38">
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>7</v>
       </c>
       <c r="B39">
-        <v>2</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="C39">
-        <v>1</v>
-      </c>
-      <c r="D39" t="s">
-        <v>12</v>
-      </c>
-      <c r="E39">
+        <v>2</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39">
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>7</v>
       </c>
       <c r="B40">
-        <v>3</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="C40">
-        <v>1</v>
-      </c>
-      <c r="D40" t="s">
-        <v>12</v>
-      </c>
-      <c r="E40">
+        <v>3</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40" t="s">
+        <v>12</v>
+      </c>
+      <c r="F40">
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>8</v>
       </c>
       <c r="B41">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="C41">
         <v>1</v>
       </c>
-      <c r="D41" t="s">
-        <v>12</v>
-      </c>
-      <c r="E41">
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41">
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>8</v>
       </c>
       <c r="B42">
-        <v>2</v>
+        <v>1.3</v>
       </c>
       <c r="C42">
-        <v>1</v>
-      </c>
-      <c r="D42" t="s">
-        <v>12</v>
-      </c>
-      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42">
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>8</v>
       </c>
       <c r="B43">
-        <v>3</v>
+        <v>1.3</v>
       </c>
       <c r="C43">
-        <v>1</v>
-      </c>
-      <c r="D43" t="s">
-        <v>12</v>
-      </c>
-      <c r="E43">
+        <v>3</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43" t="s">
+        <v>12</v>
+      </c>
+      <c r="F43">
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>2</v>
       </c>
       <c r="B44">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="C44">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D44">
+        <v>2</v>
+      </c>
+      <c r="E44">
         <v>1.23</v>
       </c>
-      <c r="E44">
+      <c r="F44">
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>2</v>
       </c>
       <c r="B45">
-        <v>2</v>
+        <v>0.4</v>
       </c>
       <c r="C45">
         <v>2</v>
       </c>
       <c r="D45">
+        <v>2</v>
+      </c>
+      <c r="E45">
         <v>1.29</v>
       </c>
-      <c r="E45">
+      <c r="F45">
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>2</v>
       </c>
       <c r="B46">
-        <v>3</v>
+        <v>0.4</v>
       </c>
       <c r="C46">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="E46">
         <v>1.72</v>
       </c>
-      <c r="E46">
+      <c r="F46">
         <v>19</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>3</v>
       </c>
       <c r="B47">
-        <v>1</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D47">
+        <v>2</v>
+      </c>
+      <c r="E47">
         <v>1.39</v>
       </c>
-      <c r="E47">
+      <c r="F47">
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>3</v>
       </c>
       <c r="B48">
-        <v>2</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C48">
         <v>2</v>
       </c>
       <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="E48">
         <v>1.42</v>
       </c>
-      <c r="E48">
+      <c r="F48">
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>3</v>
       </c>
       <c r="B49">
-        <v>3</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C49">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D49">
+        <v>2</v>
+      </c>
+      <c r="E49">
         <v>1.67</v>
       </c>
-      <c r="E49">
+      <c r="F49">
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>4</v>
       </c>
       <c r="B50">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="C50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D50">
+        <v>2</v>
+      </c>
+      <c r="E50">
         <v>1.45</v>
       </c>
-      <c r="E50">
+      <c r="F50">
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>4</v>
       </c>
       <c r="B51">
-        <v>2</v>
+        <v>0.7</v>
       </c>
       <c r="C51">
         <v>2</v>
       </c>
       <c r="D51">
+        <v>2</v>
+      </c>
+      <c r="E51">
         <v>1.27</v>
       </c>
-      <c r="E51">
+      <c r="F51">
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>4</v>
       </c>
       <c r="B52">
-        <v>3</v>
+        <v>0.7</v>
       </c>
       <c r="C52">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D52">
+        <v>2</v>
+      </c>
+      <c r="E52">
         <v>1.69</v>
       </c>
-      <c r="E52">
+      <c r="F52">
         <v>19</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>5</v>
       </c>
       <c r="B53">
-        <v>1</v>
+        <v>0.85</v>
       </c>
       <c r="C53">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D53">
+        <v>2</v>
+      </c>
+      <c r="E53">
         <v>1.75</v>
       </c>
-      <c r="E53">
+      <c r="F53">
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>5</v>
       </c>
       <c r="B54">
-        <v>2</v>
+        <v>0.85</v>
       </c>
       <c r="C54">
         <v>2</v>
       </c>
       <c r="D54">
+        <v>2</v>
+      </c>
+      <c r="E54">
         <v>1.74</v>
       </c>
-      <c r="E54">
+      <c r="F54">
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>5</v>
       </c>
       <c r="B55">
-        <v>3</v>
+        <v>0.85</v>
       </c>
       <c r="C55">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D55">
+        <v>2</v>
+      </c>
+      <c r="E55">
         <v>1.95</v>
       </c>
-      <c r="E55">
+      <c r="F55">
         <v>24</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>6</v>
       </c>
@@ -1338,356 +1506,419 @@
         <v>1</v>
       </c>
       <c r="C56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D56">
+        <v>2</v>
+      </c>
+      <c r="E56">
         <v>1.58</v>
       </c>
-      <c r="E56">
+      <c r="F56">
         <v>18</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>6</v>
       </c>
       <c r="B57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C57">
         <v>2</v>
       </c>
       <c r="D57">
+        <v>2</v>
+      </c>
+      <c r="E57">
         <v>1.55</v>
       </c>
-      <c r="E57">
+      <c r="F57">
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>6</v>
       </c>
       <c r="B58">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C58">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D58">
+        <v>2</v>
+      </c>
+      <c r="E58">
         <v>1.79</v>
       </c>
-      <c r="E58">
+      <c r="F58">
         <v>21</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>7</v>
       </c>
       <c r="B59">
-        <v>1</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="C59">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D59">
+        <v>2</v>
+      </c>
+      <c r="E59">
         <v>1.51</v>
       </c>
-      <c r="E59">
+      <c r="F59">
         <v>19</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>7</v>
       </c>
       <c r="B60">
-        <v>2</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="C60">
         <v>2</v>
       </c>
       <c r="D60">
+        <v>2</v>
+      </c>
+      <c r="E60">
         <v>1.67</v>
       </c>
-      <c r="E60">
+      <c r="F60">
         <v>21</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>7</v>
       </c>
       <c r="B61">
-        <v>3</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="C61">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D61">
+        <v>2</v>
+      </c>
+      <c r="E61">
         <v>1.53</v>
       </c>
-      <c r="E61">
+      <c r="F61">
         <v>19</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>8</v>
       </c>
       <c r="B62">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="C62">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D62">
+        <v>2</v>
+      </c>
+      <c r="E62">
         <v>1.83</v>
       </c>
-      <c r="E62">
+      <c r="F62">
         <v>28</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>8</v>
       </c>
       <c r="B63">
-        <v>2</v>
+        <v>1.3</v>
       </c>
       <c r="C63">
         <v>2</v>
       </c>
       <c r="D63">
+        <v>2</v>
+      </c>
+      <c r="E63">
         <v>1.42</v>
       </c>
-      <c r="E63">
+      <c r="F63">
         <v>18</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>8</v>
       </c>
       <c r="B64">
-        <v>3</v>
+        <v>1.3</v>
       </c>
       <c r="C64">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D64">
+        <v>2</v>
+      </c>
+      <c r="E64">
         <v>1.66</v>
       </c>
-      <c r="E64">
+      <c r="F64">
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>2</v>
       </c>
       <c r="B65">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="C65">
-        <v>3</v>
-      </c>
-      <c r="D65" t="s">
-        <v>12</v>
-      </c>
-      <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="D65">
+        <v>3</v>
+      </c>
+      <c r="E65" t="s">
+        <v>12</v>
+      </c>
+      <c r="F65">
         <v>13</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>2</v>
       </c>
       <c r="B66">
-        <v>2</v>
+        <v>0.4</v>
       </c>
       <c r="C66">
-        <v>3</v>
-      </c>
-      <c r="D66" t="s">
-        <v>12</v>
-      </c>
-      <c r="E66">
+        <v>2</v>
+      </c>
+      <c r="D66">
+        <v>3</v>
+      </c>
+      <c r="E66" t="s">
+        <v>12</v>
+      </c>
+      <c r="F66">
         <v>16</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>2</v>
       </c>
       <c r="B67">
-        <v>3</v>
+        <v>0.4</v>
       </c>
       <c r="C67">
         <v>3</v>
       </c>
-      <c r="D67" t="s">
-        <v>12</v>
-      </c>
-      <c r="E67">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D67">
+        <v>3</v>
+      </c>
+      <c r="E67" t="s">
+        <v>12</v>
+      </c>
+      <c r="F67">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>3</v>
       </c>
       <c r="B68">
-        <v>1</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C68">
-        <v>3</v>
-      </c>
-      <c r="D68" t="s">
-        <v>12</v>
-      </c>
-      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="D68">
+        <v>3</v>
+      </c>
+      <c r="E68" t="s">
+        <v>12</v>
+      </c>
+      <c r="F68">
         <v>16</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>3</v>
       </c>
       <c r="B69">
-        <v>2</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C69">
-        <v>3</v>
-      </c>
-      <c r="D69" t="s">
-        <v>12</v>
-      </c>
-      <c r="E69">
+        <v>2</v>
+      </c>
+      <c r="D69">
+        <v>3</v>
+      </c>
+      <c r="E69" t="s">
+        <v>12</v>
+      </c>
+      <c r="F69">
         <v>13</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>3</v>
       </c>
       <c r="B70">
-        <v>3</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C70">
         <v>3</v>
       </c>
-      <c r="D70" t="s">
-        <v>12</v>
-      </c>
-      <c r="E70">
+      <c r="D70">
+        <v>3</v>
+      </c>
+      <c r="E70" t="s">
+        <v>12</v>
+      </c>
+      <c r="F70">
         <v>13</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>4</v>
       </c>
       <c r="B71">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="C71">
-        <v>3</v>
-      </c>
-      <c r="D71" t="s">
-        <v>12</v>
-      </c>
-      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="D71">
+        <v>3</v>
+      </c>
+      <c r="E71" t="s">
+        <v>12</v>
+      </c>
+      <c r="F71">
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>4</v>
       </c>
       <c r="B72">
-        <v>2</v>
+        <v>0.7</v>
       </c>
       <c r="C72">
-        <v>3</v>
-      </c>
-      <c r="D72" t="s">
-        <v>12</v>
-      </c>
-      <c r="E72">
+        <v>2</v>
+      </c>
+      <c r="D72">
+        <v>3</v>
+      </c>
+      <c r="E72" t="s">
+        <v>12</v>
+      </c>
+      <c r="F72">
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>4</v>
       </c>
       <c r="B73">
-        <v>3</v>
+        <v>0.7</v>
       </c>
       <c r="C73">
         <v>3</v>
       </c>
-      <c r="D73" t="s">
-        <v>12</v>
-      </c>
-      <c r="E73">
+      <c r="D73">
+        <v>3</v>
+      </c>
+      <c r="E73" t="s">
+        <v>12</v>
+      </c>
+      <c r="F73">
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>5</v>
       </c>
       <c r="B74">
-        <v>1</v>
+        <v>0.85</v>
       </c>
       <c r="C74">
-        <v>3</v>
-      </c>
-      <c r="D74" t="s">
-        <v>12</v>
-      </c>
-      <c r="E74">
+        <v>1</v>
+      </c>
+      <c r="D74">
+        <v>3</v>
+      </c>
+      <c r="E74" t="s">
+        <v>12</v>
+      </c>
+      <c r="F74">
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>5</v>
       </c>
       <c r="B75">
-        <v>2</v>
+        <v>0.85</v>
       </c>
       <c r="C75">
-        <v>3</v>
-      </c>
-      <c r="D75" t="s">
-        <v>12</v>
-      </c>
-      <c r="E75">
+        <v>2</v>
+      </c>
+      <c r="D75">
+        <v>3</v>
+      </c>
+      <c r="E75" t="s">
+        <v>12</v>
+      </c>
+      <c r="F75">
         <v>17</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>5</v>
       </c>
       <c r="B76">
-        <v>3</v>
+        <v>0.85</v>
       </c>
       <c r="C76">
         <v>3</v>
       </c>
-      <c r="D76" t="s">
-        <v>12</v>
-      </c>
-      <c r="E76">
+      <c r="D76">
+        <v>3</v>
+      </c>
+      <c r="E76" t="s">
+        <v>12</v>
+      </c>
+      <c r="F76">
         <v>19</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>6</v>
       </c>
@@ -1695,356 +1926,419 @@
         <v>1</v>
       </c>
       <c r="C77">
-        <v>3</v>
-      </c>
-      <c r="D77" t="s">
-        <v>12</v>
-      </c>
-      <c r="E77">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+      <c r="D77">
+        <v>3</v>
+      </c>
+      <c r="E77" t="s">
+        <v>12</v>
+      </c>
+      <c r="F77">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>6</v>
       </c>
       <c r="B78">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C78">
-        <v>3</v>
-      </c>
-      <c r="D78" t="s">
-        <v>12</v>
-      </c>
-      <c r="E78">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
+        <v>2</v>
+      </c>
+      <c r="D78">
+        <v>3</v>
+      </c>
+      <c r="E78" t="s">
+        <v>12</v>
+      </c>
+      <c r="F78">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>6</v>
       </c>
       <c r="B79">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C79">
         <v>3</v>
       </c>
-      <c r="D79" t="s">
-        <v>12</v>
-      </c>
-      <c r="E79">
+      <c r="D79">
+        <v>3</v>
+      </c>
+      <c r="E79" t="s">
+        <v>12</v>
+      </c>
+      <c r="F79">
         <v>16</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>7</v>
       </c>
       <c r="B80">
-        <v>1</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="C80">
-        <v>3</v>
-      </c>
-      <c r="D80" t="s">
-        <v>12</v>
-      </c>
-      <c r="E80">
+        <v>1</v>
+      </c>
+      <c r="D80">
+        <v>3</v>
+      </c>
+      <c r="E80" t="s">
+        <v>12</v>
+      </c>
+      <c r="F80">
         <v>18</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>7</v>
       </c>
       <c r="B81">
-        <v>2</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="C81">
-        <v>3</v>
-      </c>
-      <c r="D81" t="s">
-        <v>12</v>
-      </c>
-      <c r="E81">
+        <v>2</v>
+      </c>
+      <c r="D81">
+        <v>3</v>
+      </c>
+      <c r="E81" t="s">
+        <v>12</v>
+      </c>
+      <c r="F81">
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>7</v>
       </c>
       <c r="B82">
-        <v>3</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="C82">
         <v>3</v>
       </c>
-      <c r="D82" t="s">
-        <v>12</v>
-      </c>
-      <c r="E82">
+      <c r="D82">
+        <v>3</v>
+      </c>
+      <c r="E82" t="s">
+        <v>12</v>
+      </c>
+      <c r="F82">
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>8</v>
       </c>
       <c r="B83">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="C83">
-        <v>3</v>
-      </c>
-      <c r="D83" t="s">
-        <v>12</v>
-      </c>
-      <c r="E83">
+        <v>1</v>
+      </c>
+      <c r="D83">
+        <v>3</v>
+      </c>
+      <c r="E83" t="s">
+        <v>12</v>
+      </c>
+      <c r="F83">
         <v>25</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>8</v>
       </c>
       <c r="B84">
-        <v>2</v>
+        <v>1.3</v>
       </c>
       <c r="C84">
-        <v>3</v>
-      </c>
-      <c r="D84" t="s">
-        <v>12</v>
-      </c>
-      <c r="E84">
+        <v>2</v>
+      </c>
+      <c r="D84">
+        <v>3</v>
+      </c>
+      <c r="E84" t="s">
+        <v>12</v>
+      </c>
+      <c r="F84">
         <v>14</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>8</v>
       </c>
       <c r="B85">
-        <v>3</v>
+        <v>1.3</v>
       </c>
       <c r="C85">
         <v>3</v>
       </c>
-      <c r="D85" t="s">
-        <v>12</v>
-      </c>
-      <c r="E85">
+      <c r="D85">
+        <v>3</v>
+      </c>
+      <c r="E85" t="s">
+        <v>12</v>
+      </c>
+      <c r="F85">
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>2</v>
       </c>
       <c r="B86">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="C86">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D86">
+        <v>4</v>
+      </c>
+      <c r="E86">
         <v>2.1</v>
       </c>
-      <c r="E86">
+      <c r="F86">
         <v>10</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>2</v>
       </c>
       <c r="B87">
-        <v>2</v>
+        <v>0.4</v>
       </c>
       <c r="C87">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D87">
+        <v>4</v>
+      </c>
+      <c r="E87">
         <v>2.19</v>
       </c>
-      <c r="E87">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F87">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>2</v>
       </c>
       <c r="B88">
-        <v>3</v>
+        <v>0.4</v>
       </c>
       <c r="C88">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D88">
+        <v>4</v>
+      </c>
+      <c r="E88">
         <v>1.69</v>
       </c>
-      <c r="E88">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F88">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>3</v>
       </c>
       <c r="B89">
-        <v>1</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C89">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D89">
+        <v>4</v>
+      </c>
+      <c r="E89">
         <v>2.84</v>
       </c>
-      <c r="E89">
+      <c r="F89">
         <v>13</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>3</v>
       </c>
       <c r="B90">
-        <v>2</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C90">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D90">
+        <v>4</v>
+      </c>
+      <c r="E90">
         <v>2.57</v>
       </c>
-      <c r="E90">
+      <c r="F90">
         <v>10</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>3</v>
       </c>
       <c r="B91">
-        <v>3</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C91">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D91">
+        <v>4</v>
+      </c>
+      <c r="E91">
         <v>2.44</v>
       </c>
-      <c r="E91">
+      <c r="F91">
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>4</v>
       </c>
       <c r="B92">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="C92">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D92">
+        <v>4</v>
+      </c>
+      <c r="E92">
         <v>1.8029999999999999</v>
       </c>
-      <c r="E92">
+      <c r="F92">
         <v>7</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>4</v>
       </c>
       <c r="B93">
-        <v>2</v>
+        <v>0.7</v>
       </c>
       <c r="C93">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D93">
+        <v>4</v>
+      </c>
+      <c r="E93">
         <v>2.71</v>
       </c>
-      <c r="E93">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F93">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>4</v>
       </c>
       <c r="B94">
-        <v>3</v>
+        <v>0.7</v>
       </c>
       <c r="C94">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D94">
+        <v>4</v>
+      </c>
+      <c r="E94">
         <v>3.23</v>
       </c>
-      <c r="E94">
+      <c r="F94">
         <v>13</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>5</v>
       </c>
       <c r="B95">
-        <v>1</v>
+        <v>0.85</v>
       </c>
       <c r="C95">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D95">
+        <v>4</v>
+      </c>
+      <c r="E95">
         <v>3.13</v>
       </c>
-      <c r="E95">
+      <c r="F95">
         <v>7</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>5</v>
       </c>
       <c r="B96">
-        <v>2</v>
+        <v>0.85</v>
       </c>
       <c r="C96">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D96">
+        <v>4</v>
+      </c>
+      <c r="E96">
         <v>2.67</v>
       </c>
-      <c r="E96">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F96">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>5</v>
       </c>
       <c r="B97">
-        <v>3</v>
+        <v>0.85</v>
       </c>
       <c r="C97">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D97">
+        <v>4</v>
+      </c>
+      <c r="E97">
         <v>2.81</v>
       </c>
-      <c r="E97">
+      <c r="F97">
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>6</v>
       </c>
@@ -2052,149 +2346,1016 @@
         <v>1</v>
       </c>
       <c r="C98">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D98">
+        <v>4</v>
+      </c>
+      <c r="E98">
         <v>2.5099999999999998</v>
       </c>
-      <c r="E98">
+      <c r="F98">
         <v>8</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>6</v>
       </c>
       <c r="B99">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C99">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D99">
+        <v>4</v>
+      </c>
+      <c r="E99">
         <v>2.19</v>
       </c>
-      <c r="E99">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F99">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>6</v>
       </c>
       <c r="B100">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C100">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D100">
+        <v>4</v>
+      </c>
+      <c r="E100">
         <v>2.7</v>
       </c>
-      <c r="E100">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F100">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>7</v>
       </c>
       <c r="B101">
-        <v>1</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="C101">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D101">
+        <v>4</v>
+      </c>
+      <c r="E101">
         <v>2.42</v>
       </c>
-      <c r="E101">
+      <c r="F101">
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
         <v>7</v>
       </c>
       <c r="B102">
-        <v>2</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="C102">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D102">
+        <v>4</v>
+      </c>
+      <c r="E102">
         <v>3.09</v>
       </c>
-      <c r="E102">
+      <c r="F102">
         <v>19</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>7</v>
       </c>
       <c r="B103">
-        <v>3</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="C103">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D103">
+        <v>4</v>
+      </c>
+      <c r="E103">
         <v>2.2599999999999998</v>
       </c>
-      <c r="E103">
+      <c r="F103">
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>8</v>
       </c>
       <c r="B104">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="C104">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D104">
+        <v>4</v>
+      </c>
+      <c r="E104">
         <v>2.75</v>
       </c>
-      <c r="E104">
+      <c r="F104">
         <v>18</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>8</v>
       </c>
       <c r="B105">
-        <v>2</v>
+        <v>1.3</v>
       </c>
       <c r="C105">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D105">
+        <v>4</v>
+      </c>
+      <c r="E105">
         <v>2.14</v>
       </c>
-      <c r="E105">
+      <c r="F105">
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>8</v>
       </c>
       <c r="B106">
-        <v>3</v>
+        <v>1.3</v>
       </c>
       <c r="C106">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D106">
+        <v>4</v>
+      </c>
+      <c r="E106">
         <v>3.1</v>
       </c>
-      <c r="E106">
-        <v>4</v>
+      <c r="F106">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A107" t="s">
+        <v>2</v>
+      </c>
+      <c r="B107">
+        <v>0.4</v>
+      </c>
+      <c r="C107">
+        <v>1</v>
+      </c>
+      <c r="D107">
+        <v>5</v>
+      </c>
+      <c r="E107" t="s">
+        <v>12</v>
+      </c>
+      <c r="F107">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A108" t="s">
+        <v>2</v>
+      </c>
+      <c r="B108">
+        <v>0.4</v>
+      </c>
+      <c r="C108">
+        <v>2</v>
+      </c>
+      <c r="D108">
+        <v>5</v>
+      </c>
+      <c r="E108" t="s">
+        <v>12</v>
+      </c>
+      <c r="F108">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A109" t="s">
+        <v>2</v>
+      </c>
+      <c r="B109">
+        <v>0.4</v>
+      </c>
+      <c r="C109">
+        <v>3</v>
+      </c>
+      <c r="D109">
+        <v>5</v>
+      </c>
+      <c r="E109" t="s">
+        <v>12</v>
+      </c>
+      <c r="F109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A110" t="s">
+        <v>3</v>
+      </c>
+      <c r="B110">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C110">
+        <v>1</v>
+      </c>
+      <c r="D110">
+        <v>5</v>
+      </c>
+      <c r="E110" t="s">
+        <v>12</v>
+      </c>
+      <c r="F110">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A111" t="s">
+        <v>3</v>
+      </c>
+      <c r="B111">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C111">
+        <v>2</v>
+      </c>
+      <c r="D111">
+        <v>5</v>
+      </c>
+      <c r="E111" t="s">
+        <v>12</v>
+      </c>
+      <c r="F111">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A112" t="s">
+        <v>3</v>
+      </c>
+      <c r="B112">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C112">
+        <v>3</v>
+      </c>
+      <c r="D112">
+        <v>5</v>
+      </c>
+      <c r="E112" t="s">
+        <v>12</v>
+      </c>
+      <c r="F112">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A113" t="s">
+        <v>4</v>
+      </c>
+      <c r="B113">
+        <v>0.7</v>
+      </c>
+      <c r="C113">
+        <v>1</v>
+      </c>
+      <c r="D113">
+        <v>5</v>
+      </c>
+      <c r="E113" t="s">
+        <v>12</v>
+      </c>
+      <c r="F113">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A114" t="s">
+        <v>4</v>
+      </c>
+      <c r="B114">
+        <v>0.7</v>
+      </c>
+      <c r="C114">
+        <v>2</v>
+      </c>
+      <c r="D114">
+        <v>5</v>
+      </c>
+      <c r="E114" t="s">
+        <v>12</v>
+      </c>
+      <c r="F114">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A115" t="s">
+        <v>4</v>
+      </c>
+      <c r="B115">
+        <v>0.7</v>
+      </c>
+      <c r="C115">
+        <v>3</v>
+      </c>
+      <c r="D115">
+        <v>5</v>
+      </c>
+      <c r="E115" t="s">
+        <v>12</v>
+      </c>
+      <c r="F115">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A116" t="s">
+        <v>5</v>
+      </c>
+      <c r="B116">
+        <v>0.85</v>
+      </c>
+      <c r="C116">
+        <v>1</v>
+      </c>
+      <c r="D116">
+        <v>5</v>
+      </c>
+      <c r="E116" t="s">
+        <v>12</v>
+      </c>
+      <c r="F116">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A117" t="s">
+        <v>5</v>
+      </c>
+      <c r="B117">
+        <v>0.85</v>
+      </c>
+      <c r="C117">
+        <v>2</v>
+      </c>
+      <c r="D117">
+        <v>5</v>
+      </c>
+      <c r="E117" t="s">
+        <v>12</v>
+      </c>
+      <c r="F117">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A118" t="s">
+        <v>5</v>
+      </c>
+      <c r="B118">
+        <v>0.85</v>
+      </c>
+      <c r="C118">
+        <v>3</v>
+      </c>
+      <c r="D118">
+        <v>5</v>
+      </c>
+      <c r="E118" t="s">
+        <v>12</v>
+      </c>
+      <c r="F118">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A119" t="s">
+        <v>6</v>
+      </c>
+      <c r="B119">
+        <v>1</v>
+      </c>
+      <c r="C119">
+        <v>1</v>
+      </c>
+      <c r="D119">
+        <v>5</v>
+      </c>
+      <c r="E119" t="s">
+        <v>12</v>
+      </c>
+      <c r="F119">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A120" t="s">
+        <v>6</v>
+      </c>
+      <c r="B120">
+        <v>1</v>
+      </c>
+      <c r="C120">
+        <v>2</v>
+      </c>
+      <c r="D120">
+        <v>5</v>
+      </c>
+      <c r="E120" t="s">
+        <v>12</v>
+      </c>
+      <c r="F120">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A121" t="s">
+        <v>6</v>
+      </c>
+      <c r="B121">
+        <v>1</v>
+      </c>
+      <c r="C121">
+        <v>3</v>
+      </c>
+      <c r="D121">
+        <v>5</v>
+      </c>
+      <c r="E121" t="s">
+        <v>12</v>
+      </c>
+      <c r="F121">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A122" t="s">
+        <v>7</v>
+      </c>
+      <c r="B122">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="C122">
+        <v>1</v>
+      </c>
+      <c r="D122">
+        <v>5</v>
+      </c>
+      <c r="E122" t="s">
+        <v>12</v>
+      </c>
+      <c r="F122">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A123" t="s">
+        <v>7</v>
+      </c>
+      <c r="B123">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="C123">
+        <v>2</v>
+      </c>
+      <c r="D123">
+        <v>5</v>
+      </c>
+      <c r="E123" t="s">
+        <v>12</v>
+      </c>
+      <c r="F123">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A124" t="s">
+        <v>7</v>
+      </c>
+      <c r="B124">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="C124">
+        <v>3</v>
+      </c>
+      <c r="D124">
+        <v>5</v>
+      </c>
+      <c r="E124" t="s">
+        <v>12</v>
+      </c>
+      <c r="F124">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A125" t="s">
+        <v>8</v>
+      </c>
+      <c r="B125">
+        <v>1.3</v>
+      </c>
+      <c r="C125">
+        <v>1</v>
+      </c>
+      <c r="D125">
+        <v>5</v>
+      </c>
+      <c r="E125" t="s">
+        <v>12</v>
+      </c>
+      <c r="F125">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A126" t="s">
+        <v>8</v>
+      </c>
+      <c r="B126">
+        <v>1.3</v>
+      </c>
+      <c r="C126">
+        <v>2</v>
+      </c>
+      <c r="D126">
+        <v>5</v>
+      </c>
+      <c r="E126" t="s">
+        <v>12</v>
+      </c>
+      <c r="F126">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A127" t="s">
+        <v>8</v>
+      </c>
+      <c r="B127">
+        <v>1.3</v>
+      </c>
+      <c r="C127">
+        <v>3</v>
+      </c>
+      <c r="D127">
+        <v>5</v>
+      </c>
+      <c r="E127" t="s">
+        <v>12</v>
+      </c>
+      <c r="F127">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B128">
+        <v>0.4</v>
+      </c>
+      <c r="C128">
+        <v>1</v>
+      </c>
+      <c r="D128">
+        <v>6</v>
+      </c>
+      <c r="E128">
+        <v>2.94</v>
+      </c>
+      <c r="F128">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A129" t="s">
+        <v>2</v>
+      </c>
+      <c r="B129">
+        <v>0.4</v>
+      </c>
+      <c r="C129">
+        <v>2</v>
+      </c>
+      <c r="D129">
+        <v>6</v>
+      </c>
+      <c r="E129">
+        <v>3.97</v>
+      </c>
+      <c r="F129">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A130" t="s">
+        <v>2</v>
+      </c>
+      <c r="B130">
+        <v>0.4</v>
+      </c>
+      <c r="C130">
+        <v>3</v>
+      </c>
+      <c r="D130">
+        <v>6</v>
+      </c>
+      <c r="E130">
+        <v>3.53</v>
+      </c>
+      <c r="F130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A131" t="s">
+        <v>3</v>
+      </c>
+      <c r="B131">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C131">
+        <v>1</v>
+      </c>
+      <c r="D131">
+        <v>6</v>
+      </c>
+      <c r="E131">
+        <v>4.2</v>
+      </c>
+      <c r="F131">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A132" t="s">
+        <v>3</v>
+      </c>
+      <c r="B132">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C132">
+        <v>2</v>
+      </c>
+      <c r="D132">
+        <v>6</v>
+      </c>
+      <c r="E132">
+        <v>3.23</v>
+      </c>
+      <c r="F132">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A133" t="s">
+        <v>3</v>
+      </c>
+      <c r="B133">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C133">
+        <v>3</v>
+      </c>
+      <c r="D133">
+        <v>6</v>
+      </c>
+      <c r="E133">
+        <v>2.17</v>
+      </c>
+      <c r="F133">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A134" t="s">
+        <v>4</v>
+      </c>
+      <c r="B134">
+        <v>0.7</v>
+      </c>
+      <c r="C134">
+        <v>1</v>
+      </c>
+      <c r="D134">
+        <v>6</v>
+      </c>
+      <c r="E134">
+        <v>2.09</v>
+      </c>
+      <c r="F134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A135" t="s">
+        <v>4</v>
+      </c>
+      <c r="B135">
+        <v>0.7</v>
+      </c>
+      <c r="C135">
+        <v>2</v>
+      </c>
+      <c r="D135">
+        <v>6</v>
+      </c>
+      <c r="E135">
+        <v>3.53</v>
+      </c>
+      <c r="F135">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A136" t="s">
+        <v>4</v>
+      </c>
+      <c r="B136">
+        <v>0.7</v>
+      </c>
+      <c r="C136">
+        <v>3</v>
+      </c>
+      <c r="D136">
+        <v>6</v>
+      </c>
+      <c r="E136">
+        <v>4.76</v>
+      </c>
+      <c r="F136">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A137" t="s">
+        <v>5</v>
+      </c>
+      <c r="B137">
+        <v>0.85</v>
+      </c>
+      <c r="C137">
+        <v>1</v>
+      </c>
+      <c r="D137">
+        <v>6</v>
+      </c>
+      <c r="E137">
+        <v>3.38</v>
+      </c>
+      <c r="F137">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A138" t="s">
+        <v>5</v>
+      </c>
+      <c r="B138">
+        <v>0.85</v>
+      </c>
+      <c r="C138">
+        <v>2</v>
+      </c>
+      <c r="D138">
+        <v>6</v>
+      </c>
+      <c r="E138">
+        <v>2.48</v>
+      </c>
+      <c r="F138">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A139" t="s">
+        <v>5</v>
+      </c>
+      <c r="B139">
+        <v>0.85</v>
+      </c>
+      <c r="C139">
+        <v>3</v>
+      </c>
+      <c r="D139">
+        <v>6</v>
+      </c>
+      <c r="E139">
+        <v>2.23</v>
+      </c>
+      <c r="F139">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A140" t="s">
+        <v>6</v>
+      </c>
+      <c r="B140">
+        <v>1</v>
+      </c>
+      <c r="C140">
+        <v>1</v>
+      </c>
+      <c r="D140">
+        <v>6</v>
+      </c>
+      <c r="E140">
+        <v>2.8</v>
+      </c>
+      <c r="F140">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A141" t="s">
+        <v>6</v>
+      </c>
+      <c r="B141">
+        <v>1</v>
+      </c>
+      <c r="C141">
+        <v>2</v>
+      </c>
+      <c r="D141">
+        <v>6</v>
+      </c>
+      <c r="E141">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A142" t="s">
+        <v>6</v>
+      </c>
+      <c r="B142">
+        <v>1</v>
+      </c>
+      <c r="C142">
+        <v>3</v>
+      </c>
+      <c r="D142">
+        <v>6</v>
+      </c>
+      <c r="E142">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="F142">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A143" t="s">
+        <v>7</v>
+      </c>
+      <c r="B143">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="C143">
+        <v>1</v>
+      </c>
+      <c r="D143">
+        <v>6</v>
+      </c>
+      <c r="E143">
+        <v>2.68</v>
+      </c>
+      <c r="F143">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A144" t="s">
+        <v>7</v>
+      </c>
+      <c r="B144">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="C144">
+        <v>2</v>
+      </c>
+      <c r="D144">
+        <v>6</v>
+      </c>
+      <c r="E144">
+        <v>3.14</v>
+      </c>
+      <c r="F144">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A145" t="s">
+        <v>7</v>
+      </c>
+      <c r="B145">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="C145">
+        <v>3</v>
+      </c>
+      <c r="D145">
+        <v>6</v>
+      </c>
+      <c r="E145">
+        <v>2.19</v>
+      </c>
+      <c r="F145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A146" t="s">
+        <v>8</v>
+      </c>
+      <c r="B146">
+        <v>1.3</v>
+      </c>
+      <c r="C146">
+        <v>1</v>
+      </c>
+      <c r="D146">
+        <v>6</v>
+      </c>
+      <c r="E146">
+        <v>2.41</v>
+      </c>
+      <c r="F146">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A147" t="s">
+        <v>8</v>
+      </c>
+      <c r="B147">
+        <v>1.3</v>
+      </c>
+      <c r="C147">
+        <v>2</v>
+      </c>
+      <c r="D147">
+        <v>6</v>
+      </c>
+      <c r="E147">
+        <v>2.74</v>
+      </c>
+      <c r="F147">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A148" t="s">
+        <v>8</v>
+      </c>
+      <c r="B148">
+        <v>1.3</v>
+      </c>
+      <c r="C148">
+        <v>3</v>
+      </c>
+      <c r="D148">
+        <v>6</v>
+      </c>
+      <c r="E148">
+        <v>5.23</v>
+      </c>
+      <c r="F148">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>